<commit_message>
Add many flows and handle captcha
</commit_message>
<xml_diff>
--- a/excel/test data/recharge - Copy.xlsx
+++ b/excel/test data/recharge - Copy.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA03AC6E-81FB-4D7B-BD99-899D749607DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4C182D-BD1D-4E99-B8EF-4BC221749582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30600" yWindow="1785" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="amzon recharge" sheetId="2" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +562,7 @@
         <v>6357121212</v>
       </c>
       <c r="I2">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
@@ -597,7 +597,7 @@
         <v>6357121212</v>
       </c>
       <c r="I3">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -632,7 +632,7 @@
         <v>6357121212</v>
       </c>
       <c r="I4">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -667,7 +667,7 @@
         <v>6357121212</v>
       </c>
       <c r="I5">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -702,7 +702,7 @@
         <v>6357121212</v>
       </c>
       <c r="I6">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J6" t="s">
         <v>23</v>
@@ -737,7 +737,7 @@
         <v>6357121212</v>
       </c>
       <c r="I7">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J7" t="s">
         <v>23</v>
@@ -772,7 +772,7 @@
         <v>6357121212</v>
       </c>
       <c r="I8">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J8" t="s">
         <v>23</v>
@@ -807,7 +807,7 @@
         <v>6357121212</v>
       </c>
       <c r="I9">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J9" t="s">
         <v>23</v>
@@ -842,7 +842,7 @@
         <v>6357121212</v>
       </c>
       <c r="I10">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J10" t="s">
         <v>23</v>
@@ -877,7 +877,7 @@
         <v>6357121212</v>
       </c>
       <c r="I11">
-        <v>3823330</v>
+        <v>382330</v>
       </c>
       <c r="J11" t="s">
         <v>23</v>

</xml_diff>